<commit_message>
Level 1 test case added
Level 1 test case added- space key bug
</commit_message>
<xml_diff>
--- a/Documents/Game_project_test_cases.xlsx
+++ b/Documents/Game_project_test_cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity\Final_dungeo_game\Game-Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C947D232-EF9D-4BF4-A2D2-8CADC309AC1A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817B3B70-5188-4972-8748-6BAC8D973626}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{CB8F41DC-2901-4AC8-8BB8-C04DC4CD358F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="1" xr2:uid="{CB8F41DC-2901-4AC8-8BB8-C04DC4CD358F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Test Case_ID</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Screenshot</t>
+  </si>
+  <si>
+    <t>Level 1 &gt; After pressing space button</t>
+  </si>
+  <si>
+    <t>It should attack or move forward</t>
+  </si>
+  <si>
+    <t>Charater stops at one point and doesn’t move further once pressed spacebar key</t>
   </si>
 </sst>
 </file>
@@ -111,8 +120,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F298DB-9C96-4689-A037-5B63E7DC282C}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -558,10 +570,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277BE95A-E6DE-4363-BDAC-14D12CE11B9E}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,6 +599,20 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Level 2 and Level 3 test sheet updated
Level 2 and Level 3 test sheet updated
</commit_message>
<xml_diff>
--- a/Documents/Game_project_test_cases.xlsx
+++ b/Documents/Game_project_test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity\Final_dungeo_game\Game-Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50ABF31D-4D55-4286-80C2-838890C5386A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39876A72-4E6A-41C7-B7EF-2CF9A9FA6CD2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="1" xr2:uid="{CB8F41DC-2901-4AC8-8BB8-C04DC4CD358F}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>Test Case_ID</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Rock obstacle collider</t>
   </si>
   <si>
-    <t>Canavas UI Test</t>
-  </si>
-  <si>
     <t>Help Instruction</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Level 3 Testing</t>
   </si>
   <si>
-    <t>Screenshot</t>
-  </si>
-  <si>
     <t>Level 1 &gt; After pressing space button</t>
   </si>
   <si>
@@ -100,16 +94,109 @@
   </si>
   <si>
     <t>Character is moving with low speed</t>
+  </si>
+  <si>
+    <t>TC_3</t>
+  </si>
+  <si>
+    <t>Level 1&gt; Minimap</t>
+  </si>
+  <si>
+    <t>Minimap should show in Level 1</t>
+  </si>
+  <si>
+    <t>Minimap is not showing under Level 1</t>
+  </si>
+  <si>
+    <t>TC_4</t>
+  </si>
+  <si>
+    <t>Level 1 &gt; Enemy collider</t>
+  </si>
+  <si>
+    <t>Enemy collider should work with character</t>
+  </si>
+  <si>
+    <t>Enemey collider is not working</t>
+  </si>
+  <si>
+    <t>TC_5</t>
+  </si>
+  <si>
+    <t>Level 1&gt; Weapon</t>
+  </si>
+  <si>
+    <t>Weapons needs to be added</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>More Enemy needs to be added</t>
+  </si>
+  <si>
+    <t>Functionality List</t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
+  </si>
+  <si>
+    <t>Canavas UI Design</t>
+  </si>
+  <si>
+    <t>Partially Done</t>
+  </si>
+  <si>
+    <t>In- Progress</t>
+  </si>
+  <si>
+    <t>Level 2&gt; Weapon</t>
+  </si>
+  <si>
+    <t>Level 2 &gt; Enemy collider</t>
+  </si>
+  <si>
+    <t>Level 3 &gt; Weapon</t>
+  </si>
+  <si>
+    <t>Level 3 &gt; Enemy collider</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,11 +222,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F298DB-9C96-4689-A037-5B63E7DC282C}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,125 +560,150 @@
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277BE95A-E6DE-4363-BDAC-14D12CE11B9E}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,30 +735,72 @@
     </row>
     <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -654,10 +811,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1420D960-64BC-44D7-9F39-A5329056084C}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,6 +843,34 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -693,10 +878,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CDE17B-F4E1-47BF-8E51-0555E614478C}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,6 +910,34 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Feedback from client (wallace)
Feedback from client (wallace)
</commit_message>
<xml_diff>
--- a/Documents/Game_project_test_cases.xlsx
+++ b/Documents/Game_project_test_cases.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity\Final_dungeo_game\Game-Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B75EABB-3252-4FE1-B039-4A89E9AF9077}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E38FA8-CFBF-4824-9E3D-595E91CBFBF4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{CB8F41DC-2901-4AC8-8BB8-C04DC4CD358F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="4" xr2:uid="{CB8F41DC-2901-4AC8-8BB8-C04DC4CD358F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Level 1 Testing" sheetId="2" r:id="rId2"/>
     <sheet name="Level 2 Testing" sheetId="3" r:id="rId3"/>
     <sheet name="Level 3 Testing" sheetId="4" r:id="rId4"/>
+    <sheet name="Wallace Feedback_Beta_Release" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="92">
   <si>
     <t>Test Case_ID</t>
   </si>
@@ -42,9 +43,6 @@
     <t>Actual Result</t>
   </si>
   <si>
-    <t>Developer Name</t>
-  </si>
-  <si>
     <t>Weapons needs to added</t>
   </si>
   <si>
@@ -238,6 +236,76 @@
   </si>
   <si>
     <t>Less Enemy</t>
+  </si>
+  <si>
+    <t>Some enemies (bugs) seem to move freely between a solid platform and liquid. This should be corrected to make the enemies more believable</t>
+  </si>
+  <si>
+    <t>Collider for the Enemies</t>
+  </si>
+  <si>
+    <t>AI for enemies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Also the enemies all do the exact same thing (move between 2 points). You should implement more variety such as have enemies chase the player or only move when the player is visible.Repetitive movements across multiple enemy types is lazy</t>
+  </si>
+  <si>
+    <t>Level 1 &gt; After pressing space button. Attack causes the character to spin and also prevent the player from moving at all. Given the amount of enemies in each level this is a game-breaking bug that needs to be addressed immediately.</t>
+  </si>
+  <si>
+    <t>Version history is missing descriptions of each version of the document and the changes made.</t>
+  </si>
+  <si>
+    <t>Elaborate on mechanics. "Kill enemies by attacking". Attack with what? A laser? A punch? Be specific.</t>
+  </si>
+  <si>
+    <t>ISSUE_1</t>
+  </si>
+  <si>
+    <t>ISSUE_2</t>
+  </si>
+  <si>
+    <t>ISSUE_3</t>
+  </si>
+  <si>
+    <t>ISSUE_4</t>
+  </si>
+  <si>
+    <t>ISSUE_5</t>
+  </si>
+  <si>
+    <t>ISSUE_6</t>
+  </si>
+  <si>
+    <t>Maps should have descriptions for each describing how they are each different from one another.</t>
+  </si>
+  <si>
+    <t>Visual: Document looks bland and uninspiring with only italics placed on the text. Needs more images and a unique font to make the document stand out.</t>
+  </si>
+  <si>
+    <t>ISSUE_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improvement: Looking for more improvement. Your game had a significant jump in quality from previous submissions but your document didn't receive that jump in quality.
+</t>
+  </si>
+  <si>
+    <t>Overall Feedback</t>
+  </si>
+  <si>
+    <t>Documents needs changes</t>
+  </si>
+  <si>
+    <t>Specific attack instructions need to be added after adding attack mechanism</t>
+  </si>
+  <si>
+    <t>Map descripts needs to be added under about game</t>
+  </si>
+  <si>
+    <t>Documents needs more images and unique fonts</t>
+  </si>
+  <si>
+    <t>It should attack or move forward &gt; Character stops at one point and doesn’t move further once pressed spacebar key</t>
   </si>
 </sst>
 </file>
@@ -618,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F298DB-9C96-4689-A037-5B63E7DC282C}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -634,13 +702,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -648,10 +716,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -659,10 +727,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -670,10 +738,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -681,10 +749,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -692,10 +760,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -703,10 +771,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -714,10 +782,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -725,10 +793,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -736,10 +804,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -747,10 +815,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -758,10 +826,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -775,7 +843,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,7 +856,7 @@
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,126 +870,126 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -962,92 +1030,92 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1061,7 +1129,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,95 +1155,242 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
         <v>67</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>68</v>
       </c>
-      <c r="D10" t="s">
-        <v>69</v>
-      </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05639659-9002-4383-9AD7-5004488DEEA9}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="37.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>